<commit_message>
Added Following -Json schema validation -Put, Delete(Code, no scenario) -Certificate authentication(Code, no scenario)
</commit_message>
<xml_diff>
--- a/src/test/resources/data/WebAPI_myTest.xlsx
+++ b/src/test/resources/data/WebAPI_myTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14565" windowHeight="2730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="5955" tabRatio="490" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="gitHUB" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>TestDataID</t>
   </si>
@@ -80,12 +80,6 @@
   </si>
   <si>
     <t>https://api.github.com/repos/Itsmpaul/blog/issues/2</t>
-  </si>
-  <si>
-    <t>brandDemo</t>
-  </si>
-  <si>
-    <t>Title Demo</t>
   </si>
   <si>
     <t>End to end car service validation</t>
@@ -96,6 +90,15 @@
   <si>
     <t>Content-Type:application/json
 Authorization:token TBP</t>
+  </si>
+  <si>
+    <t>AuthenticationType</t>
+  </si>
+  <si>
+    <t>AuthenticationDetails</t>
+  </si>
+  <si>
+    <t>ourTest</t>
   </si>
 </sst>
 </file>
@@ -433,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +473,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E2">
         <v>200</v>
@@ -487,10 +490,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,9 +503,10 @@
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="33.140625" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -510,7 +514,7 @@
         <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -519,31 +523,37 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -555,44 +565,46 @@
         <v>9</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>15</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f>CONCATENATE("http://localhost:3000/api/cars/",K3)</f>
+        <f>CONCATENATE("http://localhost:3000/api/cars/",M3)</f>
         <v>http://localhost:3000/api/cars/5c59157f253e4a591058bae0</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>200</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -604,19 +616,21 @@
         <v>9</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>15</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>200</v>
       </c>
     </row>

</xml_diff>